<commit_message>
Agregar talleres 3 y 4
</commit_message>
<xml_diff>
--- a/Excel clases/Evaluacion financiera de proyectos - clase.xlsx
+++ b/Excel clases/Evaluacion financiera de proyectos - clase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Finanzas Avanzadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\finanzas-avanzadas\Excel clases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAB9FE57-6AFE-4D38-B04E-33A34AAA041F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D1AB38-48E0-4E89-9F6B-D6271BC011AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B8463091-D9DC-4C29-A29E-BA5D3293FE1F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t xml:space="preserve">Periodo de Recuperación </t>
   </si>
@@ -64,13 +64,29 @@
   </si>
   <si>
     <t xml:space="preserve">4 Proyectos para evaluar: </t>
+  </si>
+  <si>
+    <t>Tasa Interna de Retorno TIRM</t>
+  </si>
+  <si>
+    <t>Años</t>
+  </si>
+  <si>
+    <t>A POS</t>
+  </si>
+  <si>
+    <t>A NEG</t>
+  </si>
+  <si>
+    <t>COC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -118,10 +134,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -437,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B40B08-AE3A-4485-890E-E49A9C133B06}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +679,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>4</v>
       </c>
@@ -669,24 +687,150 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3">
+        <v>-1500</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3">
+        <v>150</v>
+      </c>
+      <c r="D49" s="3">
+        <v>150</v>
+      </c>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50" s="3">
+        <v>1350</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1350</v>
+      </c>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" s="3">
+        <v>150</v>
+      </c>
+      <c r="D51" s="3">
+        <v>150</v>
+      </c>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52" s="3">
+        <v>-150</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53" s="3">
+        <v>-600</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3">
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D55" s="4">
+        <f>NPV(H47,D48:D53)</f>
+        <v>1364.7633358377159</v>
       </c>
     </row>
   </sheetData>
@@ -696,6 +840,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027415B4991F41841B1A250D659A23981" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="b85a395252898836deace8095741f3d3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dbbedc70-ead9-41c7-bee8-2c47823ea795" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b315d76e441ea9131fda08a2bd1c3bd3" ns3:_="">
     <xsd:import namespace="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
@@ -841,22 +1000,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2179990-7C27-4F1A-978E-FC50369F1147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6BC38D6-12DB-4518-9262-B6DF593D86B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B778BBF-E181-4801-B2BB-9186DD3067D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -872,28 +1040,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6BC38D6-12DB-4518-9262-B6DF593D86B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2179990-7C27-4F1A-978E-FC50369F1147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="dbbedc70-ead9-41c7-bee8-2c47823ea795"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>